<commit_message>
Add menu functionality for xlsx tracker
</commit_message>
<xml_diff>
--- a/admin/Menu.xlsx
+++ b/admin/Menu.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yogorus\Desktop\projects\y_lab_project\admin\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A197D7D1-1AD5-4F64-B4F1-4F7FF9BD78BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F351E9F-C16F-4FAB-BF55-FD52A41AD817}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="735" yWindow="735" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="52">
   <si>
     <t>Меню</t>
   </si>
@@ -78,109 +78,109 @@
     <t>Рамен на насыщенном сырном бульоне на основе кокосового молока, с добавлением куриной грудинки, яично - пшеничной лапши, мисо-матадоре, ростков зелени, листьев вакамэ</t>
   </si>
   <si>
+    <t>Красные вина</t>
+  </si>
+  <si>
+    <t>Для романтичного вечера</t>
+  </si>
+  <si>
+    <t>Шемен де Пап ля Ноблесс</t>
+  </si>
+  <si>
+    <t>Вино красное — фруктовое, среднетелое, выдержанное в дубе</t>
+  </si>
+  <si>
+    <t>Рипароссо Монтепульчано</t>
+  </si>
+  <si>
+    <t>Вино красное, сухое</t>
+  </si>
+  <si>
+    <t>Кьянти, Серристори</t>
+  </si>
+  <si>
+    <t>Вино красное — элегантное, комплексное, не выдержанное в дубе</t>
+  </si>
+  <si>
+    <t>Виски</t>
+  </si>
+  <si>
+    <t>Для интересных бесед</t>
+  </si>
+  <si>
+    <t>Джемисон</t>
+  </si>
+  <si>
+    <t>Классический купажированный виски, проходящий 4-хлетнюю выдержку в дубовых бочках</t>
+  </si>
+  <si>
+    <t>Джек Дэниелс</t>
+  </si>
+  <si>
+    <t>Характерен мягкий вкус, сочетает в себе карамельно-ванильные и древесные нотки. Легкий привкус дыма.</t>
+  </si>
+  <si>
+    <t>Чивас Ригал</t>
+  </si>
+  <si>
+    <t>Это купаж высококачественных солодовых и зерновых виски, выдержанных как минимум в течение 12 лет, что придает напитку роскошные нотки меда, ванили и спелых яблок.</t>
+  </si>
+  <si>
+    <t>Нарезка из ветчины, колбасных колечек, нескольких сортов сыра и фруктов</t>
+  </si>
+  <si>
+    <t>566cd1c7-455d-46f1-ac27-2dd6a0bc5915</t>
+  </si>
+  <si>
+    <t>4124c5f1-a0d6-4368-970a-f53d63987ab7</t>
+  </si>
+  <si>
+    <t>3d16522a-9884-4750-b247-2821bd49ac75</t>
+  </si>
+  <si>
+    <t>c050f03b-2cea-4269-95a8-aae0890d1bb9</t>
+  </si>
+  <si>
+    <t>14383c63-39f3-490f-adc7-701cb8d1c904</t>
+  </si>
+  <si>
+    <t>2cebddec-eb04-45c1-a163-84b1ca2c02fc</t>
+  </si>
+  <si>
+    <t>a1ff046a-676b-4967-8ee5-880a29edd0e7</t>
+  </si>
+  <si>
+    <t>959c5856-2b9b-41da-aeff-549736288140</t>
+  </si>
+  <si>
+    <t>2ed56282-aa0d-4527-8ce8-42da3c1403c1</t>
+  </si>
+  <si>
+    <t>58807647-3033-4622-80bb-962d795dea58</t>
+  </si>
+  <si>
+    <t>dc792007-676c-402b-a116-a37a57c59a6f</t>
+  </si>
+  <si>
+    <t>48ee92a9-8885-47ca-9994-c8e0fce800c4</t>
+  </si>
+  <si>
+    <t>3526363c-ee6f-4eb9-93f2-665ba58496bf</t>
+  </si>
+  <si>
+    <t>86cdee11-411a-4ea8-860a-c9ead273a914</t>
+  </si>
+  <si>
+    <t>3989e1ec-ad34-4458-85af-c749c8fa8543</t>
+  </si>
+  <si>
+    <t>4bbdad9c-83a1-4410-bd98-e2a22ee42e93</t>
+  </si>
+  <si>
     <t>Алкогольное меню</t>
   </si>
   <si>
     <t>Алкогольные напитки</t>
-  </si>
-  <si>
-    <t>Красные вина</t>
-  </si>
-  <si>
-    <t>Для романтичного вечера</t>
-  </si>
-  <si>
-    <t>Шемен де Пап ля Ноблесс</t>
-  </si>
-  <si>
-    <t>Вино красное — фруктовое, среднетелое, выдержанное в дубе</t>
-  </si>
-  <si>
-    <t>Рипароссо Монтепульчано</t>
-  </si>
-  <si>
-    <t>Вино красное, сухое</t>
-  </si>
-  <si>
-    <t>Кьянти, Серристори</t>
-  </si>
-  <si>
-    <t>Вино красное — элегантное, комплексное, не выдержанное в дубе</t>
-  </si>
-  <si>
-    <t>Виски</t>
-  </si>
-  <si>
-    <t>Для интересных бесед</t>
-  </si>
-  <si>
-    <t>Джемисон</t>
-  </si>
-  <si>
-    <t>Классический купажированный виски, проходящий 4-хлетнюю выдержку в дубовых бочках</t>
-  </si>
-  <si>
-    <t>Джек Дэниелс</t>
-  </si>
-  <si>
-    <t>Характерен мягкий вкус, сочетает в себе карамельно-ванильные и древесные нотки. Легкий привкус дыма.</t>
-  </si>
-  <si>
-    <t>Чивас Ригал</t>
-  </si>
-  <si>
-    <t>Это купаж высококачественных солодовых и зерновых виски, выдержанных как минимум в течение 12 лет, что придает напитку роскошные нотки меда, ванили и спелых яблок.</t>
-  </si>
-  <si>
-    <t>Нарезка из ветчины, колбасных колечек, нескольких сортов сыра и фруктов</t>
-  </si>
-  <si>
-    <t>566cd1c7-455d-46f1-ac27-2dd6a0bc5915</t>
-  </si>
-  <si>
-    <t>4124c5f1-a0d6-4368-970a-f53d63987ab7</t>
-  </si>
-  <si>
-    <t>3d16522a-9884-4750-b247-2821bd49ac75</t>
-  </si>
-  <si>
-    <t>c050f03b-2cea-4269-95a8-aae0890d1bb9</t>
-  </si>
-  <si>
-    <t>14383c63-39f3-490f-adc7-701cb8d1c904</t>
-  </si>
-  <si>
-    <t>2cebddec-eb04-45c1-a163-84b1ca2c02fc</t>
-  </si>
-  <si>
-    <t>a1ff046a-676b-4967-8ee5-880a29edd0e7</t>
-  </si>
-  <si>
-    <t>959c5856-2b9b-41da-aeff-549736288140</t>
-  </si>
-  <si>
-    <t>2ed56282-aa0d-4527-8ce8-42da3c1403c1</t>
-  </si>
-  <si>
-    <t>58807647-3033-4622-80bb-962d795dea58</t>
-  </si>
-  <si>
-    <t>dc792007-676c-402b-a116-a37a57c59a6f</t>
-  </si>
-  <si>
-    <t>48ee92a9-8885-47ca-9994-c8e0fce800c4</t>
-  </si>
-  <si>
-    <t>3526363c-ee6f-4eb9-93f2-665ba58496bf</t>
-  </si>
-  <si>
-    <t>86cdee11-411a-4ea8-860a-c9ead273a914</t>
-  </si>
-  <si>
-    <t>3989e1ec-ad34-4458-85af-c749c8fa8543</t>
-  </si>
-  <si>
-    <t>4bbdad9c-83a1-4410-bd98-e2a22ee42e93</t>
   </si>
 </sst>
 </file>
@@ -485,10 +485,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:F1000"/>
+  <dimension ref="A1:F999"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -496,14 +496,14 @@
     <col min="1" max="1" width="47.85546875" customWidth="1"/>
     <col min="2" max="2" width="48.5703125" customWidth="1"/>
     <col min="3" max="3" width="54.140625" customWidth="1"/>
-    <col min="4" max="4" width="21.7109375" style="9" customWidth="1"/>
+    <col min="4" max="4" width="31.28515625" style="9" customWidth="1"/>
     <col min="5" max="5" width="77.7109375" style="9" customWidth="1"/>
     <col min="6" max="6" width="12.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -515,10 +515,10 @@
       <c r="E1" s="8"/>
       <c r="F1" s="2"/>
     </row>
-    <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="2"/>
       <c r="B2" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>2</v>
@@ -533,7 +533,7 @@
       <c r="A3" s="2"/>
       <c r="B3" s="1"/>
       <c r="C3" s="10" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D3" s="8" t="s">
         <v>4</v>
@@ -549,13 +549,13 @@
       <c r="A4" s="2"/>
       <c r="B4" s="1"/>
       <c r="C4" s="10" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D4" s="8" t="s">
         <v>6</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="F4" s="4">
         <v>215.36</v>
@@ -565,7 +565,7 @@
       <c r="A5" s="2"/>
       <c r="B5" s="1"/>
       <c r="C5" s="10" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D5" s="8" t="s">
         <v>7</v>
@@ -580,7 +580,7 @@
     <row r="6" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="2"/>
       <c r="B6" s="10" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>9</v>
@@ -595,7 +595,7 @@
       <c r="A7" s="2"/>
       <c r="B7" s="2"/>
       <c r="C7" s="10" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D7" s="8" t="s">
         <v>11</v>
@@ -611,7 +611,7 @@
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
       <c r="C8" s="10" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D8" s="8" t="s">
         <v>13</v>
@@ -627,7 +627,7 @@
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" s="10" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D9" s="8" t="s">
         <v>15</v>
@@ -639,30 +639,30 @@
         <v>132.88</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="5" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>17</v>
+        <v>50</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>18</v>
+        <v>51</v>
       </c>
       <c r="D10" s="8"/>
       <c r="E10" s="7"/>
       <c r="F10" s="2"/>
     </row>
-    <row r="11" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="2"/>
       <c r="B11" s="1">
         <v>1</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E11" s="7"/>
       <c r="F11" s="2"/>
@@ -671,13 +671,13 @@
       <c r="A12" s="2"/>
       <c r="B12" s="1"/>
       <c r="C12" s="10" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E12" s="7" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="F12" s="1">
         <v>2700.79</v>
@@ -687,13 +687,13 @@
       <c r="A13" s="2"/>
       <c r="B13" s="1"/>
       <c r="C13" s="10" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E13" s="7" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="F13" s="1">
         <v>3100.33</v>
@@ -703,28 +703,28 @@
       <c r="A14" s="2"/>
       <c r="B14" s="1"/>
       <c r="C14" s="10" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E14" s="7" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="F14" s="1">
         <v>1850.42</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="2"/>
       <c r="B15" s="1">
         <v>2</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="E15" s="7"/>
       <c r="F15" s="2"/>
@@ -733,13 +733,13 @@
       <c r="A16" s="2"/>
       <c r="B16" s="2"/>
       <c r="C16" s="10" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E16" s="7" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F16" s="1">
         <v>420.78</v>
@@ -749,13 +749,13 @@
       <c r="A17" s="2"/>
       <c r="B17" s="2"/>
       <c r="C17" s="10" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D17" s="8" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E17" s="7" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="F17" s="1">
         <v>440.11</v>
@@ -765,13 +765,13 @@
       <c r="A18" s="2"/>
       <c r="B18" s="2"/>
       <c r="C18" s="10" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D18" s="8" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E18" s="7" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="F18" s="1">
         <v>520.08000000000004</v>
@@ -1758,7 +1758,6 @@
     <row r="997" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="998" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="999" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="1000" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
add working excel celery task
</commit_message>
<xml_diff>
--- a/admin/Menu.xlsx
+++ b/admin/Menu.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yogorus\Desktop\projects\y_lab_project\admin\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F351E9F-C16F-4FAB-BF55-FD52A41AD817}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32DB3341-1290-4B11-B1B2-AED9C8776B5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="735" yWindow="735" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="1095" windowWidth="27090" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="54">
   <si>
     <t>Меню</t>
   </si>
@@ -36,151 +36,157 @@
     <t>Холодные закуски</t>
   </si>
   <si>
+    <t>Сельдь Бисмарк</t>
+  </si>
+  <si>
+    <t>Традиционное немецкое блюдо из маринованной сельди</t>
+  </si>
+  <si>
+    <t>Мясная тарелка</t>
+  </si>
+  <si>
+    <t>Рыбная тарелка</t>
+  </si>
+  <si>
+    <t>Нарезка из креветок, кальмаров, раковых шеек, гребешков, лосося, скумбрии и красной икры</t>
+  </si>
+  <si>
+    <t>Горячий рамен</t>
+  </si>
+  <si>
+    <t>Дайзу рамен</t>
+  </si>
+  <si>
+    <t>Рамен на курином бульоне с куриными подушками и яйцом аджитама, яично-пшеничной лапшой, ростки зелени, грибами муэр и зеленым луком</t>
+  </si>
+  <si>
+    <t>Унаги рамен</t>
+  </si>
+  <si>
+    <t>Рамен на нежном сливочном рыбном бульоне, с добавлением маринованного угря, грибов муэр, кунжута, зеленого лука</t>
+  </si>
+  <si>
+    <t>Чиизу Рамен</t>
+  </si>
+  <si>
+    <t>Рамен на насыщенном сырном бульоне на основе кокосового молока, с добавлением куриной грудинки, яично - пшеничной лапши, мисо-матадоре, ростков зелени, листьев вакамэ</t>
+  </si>
+  <si>
+    <t>Красные вина</t>
+  </si>
+  <si>
+    <t>Для романтичного вечера</t>
+  </si>
+  <si>
+    <t>Шемен де Пап ля Ноблесс</t>
+  </si>
+  <si>
+    <t>Вино красное — фруктовое, среднетелое, выдержанное в дубе</t>
+  </si>
+  <si>
+    <t>Рипароссо Монтепульчано</t>
+  </si>
+  <si>
+    <t>Вино красное, сухое</t>
+  </si>
+  <si>
+    <t>Кьянти, Серристори</t>
+  </si>
+  <si>
+    <t>Вино красное — элегантное, комплексное, не выдержанное в дубе</t>
+  </si>
+  <si>
+    <t>Для интересных бесед</t>
+  </si>
+  <si>
+    <t>Джемисон</t>
+  </si>
+  <si>
+    <t>Классический купажированный виски, проходящий 4-хлетнюю выдержку в дубовых бочках</t>
+  </si>
+  <si>
+    <t>Джек Дэниелс</t>
+  </si>
+  <si>
+    <t>Характерен мягкий вкус, сочетает в себе карамельно-ванильные и древесные нотки. Легкий привкус дыма.</t>
+  </si>
+  <si>
+    <t>Чивас Ригал</t>
+  </si>
+  <si>
+    <t>Это купаж высококачественных солодовых и зерновых виски, выдержанных как минимум в течение 12 лет, что придает напитку роскошные нотки меда, ванили и спелых яблок.</t>
+  </si>
+  <si>
+    <t>Нарезка из ветчины, колбасных колечек, нескольких сортов сыра и фруктов</t>
+  </si>
+  <si>
+    <t>566cd1c7-455d-46f1-ac27-2dd6a0bc5915</t>
+  </si>
+  <si>
+    <t>4124c5f1-a0d6-4368-970a-f53d63987ab7</t>
+  </si>
+  <si>
+    <t>3d16522a-9884-4750-b247-2821bd49ac75</t>
+  </si>
+  <si>
+    <t>c050f03b-2cea-4269-95a8-aae0890d1bb9</t>
+  </si>
+  <si>
+    <t>14383c63-39f3-490f-adc7-701cb8d1c904</t>
+  </si>
+  <si>
+    <t>2cebddec-eb04-45c1-a163-84b1ca2c02fc</t>
+  </si>
+  <si>
+    <t>a1ff046a-676b-4967-8ee5-880a29edd0e7</t>
+  </si>
+  <si>
+    <t>959c5856-2b9b-41da-aeff-549736288140</t>
+  </si>
+  <si>
+    <t>2ed56282-aa0d-4527-8ce8-42da3c1403c1</t>
+  </si>
+  <si>
+    <t>58807647-3033-4622-80bb-962d795dea58</t>
+  </si>
+  <si>
+    <t>dc792007-676c-402b-a116-a37a57c59a6f</t>
+  </si>
+  <si>
+    <t>48ee92a9-8885-47ca-9994-c8e0fce800c4</t>
+  </si>
+  <si>
+    <t>3526363c-ee6f-4eb9-93f2-665ba58496bf</t>
+  </si>
+  <si>
+    <t>86cdee11-411a-4ea8-860a-c9ead273a914</t>
+  </si>
+  <si>
+    <t>3989e1ec-ad34-4458-85af-c749c8fa8543</t>
+  </si>
+  <si>
+    <t>4bbdad9c-83a1-4410-bd98-e2a22ee42e93</t>
+  </si>
+  <si>
+    <t>Алкогольное меню</t>
+  </si>
+  <si>
+    <t>Алкогольные напитки</t>
+  </si>
+  <si>
+    <t>66efffda-25ca-4219-aceb-44bd8758e2d7</t>
+  </si>
+  <si>
+    <t>edb8f441-e0cf-4b5b-a9ce-f42160f86f7a</t>
+  </si>
+  <si>
+    <t>Рамен</t>
+  </si>
+  <si>
+    <t>Виски</t>
+  </si>
+  <si>
     <t>К пиву</t>
-  </si>
-  <si>
-    <t>Сельдь Бисмарк</t>
-  </si>
-  <si>
-    <t>Традиционное немецкое блюдо из маринованной сельди</t>
-  </si>
-  <si>
-    <t>Мясная тарелка</t>
-  </si>
-  <si>
-    <t>Рыбная тарелка</t>
-  </si>
-  <si>
-    <t>Нарезка из креветок, кальмаров, раковых шеек, гребешков, лосося, скумбрии и красной икры</t>
-  </si>
-  <si>
-    <t>Рамен</t>
-  </si>
-  <si>
-    <t>Горячий рамен</t>
-  </si>
-  <si>
-    <t>Дайзу рамен</t>
-  </si>
-  <si>
-    <t>Рамен на курином бульоне с куриными подушками и яйцом аджитама, яично-пшеничной лапшой, ростки зелени, грибами муэр и зеленым луком</t>
-  </si>
-  <si>
-    <t>Унаги рамен</t>
-  </si>
-  <si>
-    <t>Рамен на нежном сливочном рыбном бульоне, с добавлением маринованного угря, грибов муэр, кунжута, зеленого лука</t>
-  </si>
-  <si>
-    <t>Чиизу Рамен</t>
-  </si>
-  <si>
-    <t>Рамен на насыщенном сырном бульоне на основе кокосового молока, с добавлением куриной грудинки, яично - пшеничной лапши, мисо-матадоре, ростков зелени, листьев вакамэ</t>
-  </si>
-  <si>
-    <t>Красные вина</t>
-  </si>
-  <si>
-    <t>Для романтичного вечера</t>
-  </si>
-  <si>
-    <t>Шемен де Пап ля Ноблесс</t>
-  </si>
-  <si>
-    <t>Вино красное — фруктовое, среднетелое, выдержанное в дубе</t>
-  </si>
-  <si>
-    <t>Рипароссо Монтепульчано</t>
-  </si>
-  <si>
-    <t>Вино красное, сухое</t>
-  </si>
-  <si>
-    <t>Кьянти, Серристори</t>
-  </si>
-  <si>
-    <t>Вино красное — элегантное, комплексное, не выдержанное в дубе</t>
-  </si>
-  <si>
-    <t>Виски</t>
-  </si>
-  <si>
-    <t>Для интересных бесед</t>
-  </si>
-  <si>
-    <t>Джемисон</t>
-  </si>
-  <si>
-    <t>Классический купажированный виски, проходящий 4-хлетнюю выдержку в дубовых бочках</t>
-  </si>
-  <si>
-    <t>Джек Дэниелс</t>
-  </si>
-  <si>
-    <t>Характерен мягкий вкус, сочетает в себе карамельно-ванильные и древесные нотки. Легкий привкус дыма.</t>
-  </si>
-  <si>
-    <t>Чивас Ригал</t>
-  </si>
-  <si>
-    <t>Это купаж высококачественных солодовых и зерновых виски, выдержанных как минимум в течение 12 лет, что придает напитку роскошные нотки меда, ванили и спелых яблок.</t>
-  </si>
-  <si>
-    <t>Нарезка из ветчины, колбасных колечек, нескольких сортов сыра и фруктов</t>
-  </si>
-  <si>
-    <t>566cd1c7-455d-46f1-ac27-2dd6a0bc5915</t>
-  </si>
-  <si>
-    <t>4124c5f1-a0d6-4368-970a-f53d63987ab7</t>
-  </si>
-  <si>
-    <t>3d16522a-9884-4750-b247-2821bd49ac75</t>
-  </si>
-  <si>
-    <t>c050f03b-2cea-4269-95a8-aae0890d1bb9</t>
-  </si>
-  <si>
-    <t>14383c63-39f3-490f-adc7-701cb8d1c904</t>
-  </si>
-  <si>
-    <t>2cebddec-eb04-45c1-a163-84b1ca2c02fc</t>
-  </si>
-  <si>
-    <t>a1ff046a-676b-4967-8ee5-880a29edd0e7</t>
-  </si>
-  <si>
-    <t>959c5856-2b9b-41da-aeff-549736288140</t>
-  </si>
-  <si>
-    <t>2ed56282-aa0d-4527-8ce8-42da3c1403c1</t>
-  </si>
-  <si>
-    <t>58807647-3033-4622-80bb-962d795dea58</t>
-  </si>
-  <si>
-    <t>dc792007-676c-402b-a116-a37a57c59a6f</t>
-  </si>
-  <si>
-    <t>48ee92a9-8885-47ca-9994-c8e0fce800c4</t>
-  </si>
-  <si>
-    <t>3526363c-ee6f-4eb9-93f2-665ba58496bf</t>
-  </si>
-  <si>
-    <t>86cdee11-411a-4ea8-860a-c9ead273a914</t>
-  </si>
-  <si>
-    <t>3989e1ec-ad34-4458-85af-c749c8fa8543</t>
-  </si>
-  <si>
-    <t>4bbdad9c-83a1-4410-bd98-e2a22ee42e93</t>
-  </si>
-  <si>
-    <t>Алкогольное меню</t>
-  </si>
-  <si>
-    <t>Алкогольные напитки</t>
   </si>
 </sst>
 </file>
@@ -488,7 +494,7 @@
   <dimension ref="A1:F999"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -497,13 +503,13 @@
     <col min="2" max="2" width="48.5703125" customWidth="1"/>
     <col min="3" max="3" width="54.140625" customWidth="1"/>
     <col min="4" max="4" width="31.28515625" style="9" customWidth="1"/>
-    <col min="5" max="5" width="77.7109375" style="9" customWidth="1"/>
+    <col min="5" max="5" width="83.42578125" style="9" customWidth="1"/>
     <col min="6" max="6" width="12.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -518,13 +524,13 @@
     <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="2"/>
       <c r="B2" s="3" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>3</v>
+        <v>53</v>
       </c>
       <c r="E2" s="8"/>
       <c r="F2" s="2"/>
@@ -533,13 +539,13 @@
       <c r="A3" s="2"/>
       <c r="B3" s="1"/>
       <c r="C3" s="10" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="D3" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" s="7" t="s">
         <v>4</v>
-      </c>
-      <c r="E3" s="7" t="s">
-        <v>5</v>
       </c>
       <c r="F3" s="4">
         <v>182.99</v>
@@ -549,13 +555,13 @@
       <c r="A4" s="2"/>
       <c r="B4" s="1"/>
       <c r="C4" s="10" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="F4" s="4">
         <v>215.36</v>
@@ -565,13 +571,13 @@
       <c r="A5" s="2"/>
       <c r="B5" s="1"/>
       <c r="C5" s="10" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="D5" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="E5" s="7" t="s">
         <v>7</v>
-      </c>
-      <c r="E5" s="7" t="s">
-        <v>8</v>
       </c>
       <c r="F5" s="4">
         <v>265.57</v>
@@ -580,13 +586,13 @@
     <row r="6" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="2"/>
       <c r="B6" s="10" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>9</v>
+        <v>51</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E6" s="7"/>
       <c r="F6" s="2"/>
@@ -595,13 +601,13 @@
       <c r="A7" s="2"/>
       <c r="B7" s="2"/>
       <c r="C7" s="10" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F7" s="1">
         <v>166.47</v>
@@ -611,13 +617,13 @@
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
       <c r="C8" s="10" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="F8" s="1">
         <v>168.25</v>
@@ -627,13 +633,13 @@
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" s="10" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="F9" s="1">
         <v>132.88</v>
@@ -641,13 +647,13 @@
     </row>
     <row r="10" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="5" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="D10" s="8"/>
       <c r="E10" s="7"/>
@@ -655,29 +661,29 @@
     </row>
     <row r="11" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="2"/>
-      <c r="B11" s="1">
-        <v>1</v>
+      <c r="B11" s="3" t="s">
+        <v>49</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E11" s="7"/>
       <c r="F11" s="2"/>
     </row>
     <row r="12" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="2"/>
-      <c r="B12" s="1"/>
+      <c r="B12" s="3"/>
       <c r="C12" s="10" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E12" s="7" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="F12" s="1">
         <v>2700.79</v>
@@ -685,15 +691,15 @@
     </row>
     <row r="13" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="2"/>
-      <c r="B13" s="1"/>
+      <c r="B13" s="3"/>
       <c r="C13" s="10" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E13" s="7" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="F13" s="1">
         <v>3100.33</v>
@@ -701,15 +707,15 @@
     </row>
     <row r="14" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="2"/>
-      <c r="B14" s="1"/>
+      <c r="B14" s="3"/>
       <c r="C14" s="10" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E14" s="7" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="F14" s="1">
         <v>1850.42</v>
@@ -717,14 +723,14 @@
     </row>
     <row r="15" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="2"/>
-      <c r="B15" s="1">
-        <v>2</v>
+      <c r="B15" s="3" t="s">
+        <v>50</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>25</v>
+        <v>52</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="E15" s="7"/>
       <c r="F15" s="2"/>
@@ -733,13 +739,13 @@
       <c r="A16" s="2"/>
       <c r="B16" s="2"/>
       <c r="C16" s="10" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="E16" s="7" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="F16" s="1">
         <v>420.78</v>
@@ -749,13 +755,13 @@
       <c r="A17" s="2"/>
       <c r="B17" s="2"/>
       <c r="C17" s="10" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="D17" s="8" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="E17" s="7" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="F17" s="1">
         <v>440.11</v>
@@ -765,21 +771,30 @@
       <c r="A18" s="2"/>
       <c r="B18" s="2"/>
       <c r="C18" s="10" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D18" s="8" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="E18" s="7" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="F18" s="1">
         <v>520.08000000000004</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="20" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="21" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="19" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D19"/>
+      <c r="E19"/>
+    </row>
+    <row r="20" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D20"/>
+      <c r="E20"/>
+    </row>
+    <row r="21" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D21"/>
+      <c r="E21"/>
+    </row>
     <row r="22" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="23" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="24" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
add background tasks cache invalidation in menu
</commit_message>
<xml_diff>
--- a/admin/Menu.xlsx
+++ b/admin/Menu.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yogorus\Desktop\projects\y_lab_project\admin\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32DB3341-1290-4B11-B1B2-AED9C8776B5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F9688EE-7A37-47F7-BECE-7F63EFB14361}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="1095" windowWidth="27090" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -494,7 +494,7 @@
   <dimension ref="A1:F999"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="F18" sqref="A10:F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
fix celery submenu deletion
</commit_message>
<xml_diff>
--- a/admin/Menu.xlsx
+++ b/admin/Menu.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yogorus\Desktop\projects\y_lab_project\admin\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F9688EE-7A37-47F7-BECE-7F63EFB14361}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9F3CB74-0E44-423C-B9FC-6C1CD3749CA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="1095" windowWidth="27090" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -494,7 +494,7 @@
   <dimension ref="A1:F999"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="F18" sqref="A10:F18"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>